<commit_message>
all new writers added
</commit_message>
<xml_diff>
--- a/Smart Urdu Novel Bank/add_new_novel.xlsx
+++ b/Smart Urdu Novel Bank/add_new_novel.xlsx
@@ -27,12 +27,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Titles</t>
   </si>
   <si>
     <t>Links</t>
+  </si>
+  <si>
+    <t>Ankaboot novel by noor rajpoot (complete)</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1dqUYRA55rb8q-rWk9NZI7P6Ck8GzTmVr</t>
+  </si>
+  <si>
+    <t>Lohe Mehfooz Novel</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1EhbBud6TX1iFtXQ8FLIQX5k4GchP7Myu</t>
+  </si>
+  <si>
+    <t>Zakham e zeest by Haleema Sadia</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1D_DYk33DyRXoEUC7NQAa2UZqdYG5ZAef</t>
+  </si>
+  <si>
+    <t>Dastan e firaq by Haleema Sadia</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1bU8hq3KmBr1hUhLW73ixWO9DG6vtDJiN/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Akhari Barsat novel by sameera khan</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1suVH73KWVrljwDaseIHmF5u09zk0__h0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Qalbe munqalib novel by aina noor</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1Gznt84VX-GZlnmXXHOS-l9TG4kMv7olT</t>
+  </si>
+  <si>
+    <t>Bharam Baqa Umeed by Mehrunisa Shahmeer</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1w0V4qti7ZwjjrcZSDaQr1uuo0VCVOA5i</t>
+  </si>
+  <si>
+    <t>Hameesha Ka Mehman By Asad ali</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/07/hameesha-ka-mehman-afsana-by-asad-ali.html</t>
+  </si>
+  <si>
+    <t>Jaray Ki Chandni By Sikandar Malik</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/07/jaray-ki-chandni-novel-by-sikandar-malik.html</t>
+  </si>
+  <si>
+    <t>Main bhi insan hun by fatima</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/07/main-bhi-insan-hun-novel-by-fatima.html</t>
+  </si>
+  <si>
+    <t>Anjan Safar Anjan Rahi by Tayyaba Imran</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1oJpAyLaoqRcLjfsyd1VIXMXvmA1OBIyR</t>
+  </si>
+  <si>
+    <t>Hikmat ilahi novel by tayyaba imran</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15Sg5Bd7UKbYwb7VNP8EfvJXgMcwIrGQl/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Velutha Novel by rabia khan</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1zSpbrZuE4iyC6zD_Ae6mwPSNQxMSD1Th</t>
+  </si>
+  <si>
+    <t>Jab Jang hoti ha by fatima</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/05/jab-jang-hoti-ha-by-fatima.html</t>
+  </si>
+  <si>
+    <t>Bar aks novel by sikandar malik</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/02/bar-aks-novel-by-sikander-malik.html</t>
+  </si>
+  <si>
+    <t>Con Amore By sahab khan</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/01/con-amore-novel-by-sahab-khan.html</t>
+  </si>
+  <si>
+    <t>Qissa e dard novel by Irza khan</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2025/01/qissa-e-dard-novel-by-irza-khan.html</t>
+  </si>
+  <si>
+    <t>Qeemti Mohabbat novel by Nasreen Ameer ali</t>
+  </si>
+  <si>
+    <t>https://www.urdunovelbanks.com/2024/09/qeemti-mohabbat-novel-by-nasreen-ameer.html</t>
   </si>
 </sst>
 </file>
@@ -646,9 +754,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,13 +1078,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="47.3636363636364" customWidth="1"/>
     <col min="2" max="2" width="51.4545454545455" customWidth="1"/>
@@ -988,10 +1098,160 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://drive.google.com/drive/folders/1dqUYRA55rb8q-rWk9NZI7P6Ck8GzTmVr"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://drive.google.com/drive/folders/1EhbBud6TX1iFtXQ8FLIQX5k4GchP7Myu"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://drive.google.com/drive/folders/1D_DYk33DyRXoEUC7NQAa2UZqdYG5ZAef" tooltip="https://drive.google.com/drive/folders/1D_DYk33DyRXoEUC7NQAa2UZqdYG5ZAef"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://drive.google.com/file/d/1bU8hq3KmBr1hUhLW73ixWO9DG6vtDJiN/view?usp=sharing" tooltip="https://drive.google.com/file/d/1bU8hq3KmBr1hUhLW73ixWO9DG6vtDJiN/view?usp=sharing"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://drive.google.com/file/d/1suVH73KWVrljwDaseIHmF5u09zk0__h0/view?usp=sharing"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://drive.google.com/drive/folders/1Gznt84VX-GZlnmXXHOS-l9TG4kMv7olT"/>
+    <hyperlink ref="B13" r:id="rId7" display="https://drive.google.com/file/d/15Sg5Bd7UKbYwb7VNP8EfvJXgMcwIrGQl/view?usp=sharing"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>